<commit_message>
sự kiện phims enter . Xuất hóa đoưn PDF.....
</commit_message>
<xml_diff>
--- a/DSHoaDon.xlsx
+++ b/DSHoaDon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Mã HD</t>
   </si>
@@ -44,6 +44,9 @@
     <t>NV001</t>
   </si>
   <si>
+    <t>KM001</t>
+  </si>
+  <si>
     <t>HD002</t>
   </si>
   <si>
@@ -87,6 +90,39 @@
   </si>
   <si>
     <t>KM004</t>
+  </si>
+  <si>
+    <t>HD005</t>
+  </si>
+  <si>
+    <t>2023-12-08</t>
+  </si>
+  <si>
+    <t>KH040</t>
+  </si>
+  <si>
+    <t>nullKM001,</t>
+  </si>
+  <si>
+    <t>HD006</t>
+  </si>
+  <si>
+    <t>2023-12-09</t>
+  </si>
+  <si>
+    <t>HD007</t>
+  </si>
+  <si>
+    <t>HD008</t>
+  </si>
+  <si>
+    <t>HD009</t>
+  </si>
+  <si>
+    <t>HD010</t>
+  </si>
+  <si>
+    <t>KM001,</t>
   </si>
 </sst>
 </file>
@@ -131,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -170,26 +206,28 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2"/>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" t="n">
         <v>1000000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="n">
         <v>1500000.0</v>
@@ -197,19 +235,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" t="n">
         <v>800000.0</v>
@@ -217,22 +255,142 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="n">
         <v>1200000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="n">
+        <v>100000.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="n">
+        <v>100000.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="n">
+        <v>100000.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="n">
+        <v>420000.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="n">
+        <v>100000.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="n">
+        <v>100000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cập nhật giao diện
</commit_message>
<xml_diff>
--- a/DSHoaDon.xlsx
+++ b/DSHoaDon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Mã HD</t>
   </si>
@@ -44,6 +44,9 @@
     <t>NV001</t>
   </si>
   <si>
+    <t>KM001</t>
+  </si>
+  <si>
     <t>HD002</t>
   </si>
   <si>
@@ -87,6 +90,27 @@
   </si>
   <si>
     <t>KM004</t>
+  </si>
+  <si>
+    <t>HD005</t>
+  </si>
+  <si>
+    <t>2023-12-09</t>
+  </si>
+  <si>
+    <t>KH041</t>
+  </si>
+  <si>
+    <t>KM001,</t>
+  </si>
+  <si>
+    <t>HD006</t>
+  </si>
+  <si>
+    <t>HD007</t>
+  </si>
+  <si>
+    <t>HD008</t>
   </si>
 </sst>
 </file>
@@ -131,7 +155,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -170,26 +194,28 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2"/>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" t="n">
         <v>1000000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="n">
         <v>1500000.0</v>
@@ -197,19 +223,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" t="n">
         <v>800000.0</v>
@@ -217,22 +243,96 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="n">
         <v>1200000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="n">
+        <v>298000.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>